<commit_message>
refactor: dong vat, cham soc, ncc, thucan,.. update: database
</commit_message>
<xml_diff>
--- a/export/ChuongTrai.xlsx
+++ b/export/ChuongTrai.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Mã</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Số lượng tối đa</t>
   </si>
   <si>
+    <t>Ảnh</t>
+  </si>
+  <si>
     <t>57</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
     <t>5</t>
   </si>
   <si>
+    <t>BaoHabitat.jpg</t>
+  </si>
+  <si>
     <t>58</t>
   </si>
   <si>
@@ -56,6 +62,9 @@
     <t>7</t>
   </si>
   <si>
+    <t>ChimCongHabitat.jpg</t>
+  </si>
+  <si>
     <t>60</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
     <t>6</t>
   </si>
   <si>
+    <t>VoiHabitat.jpg</t>
+  </si>
+  <si>
     <t>62</t>
   </si>
   <si>
@@ -83,6 +95,9 @@
     <t>4</t>
   </si>
   <si>
+    <t>CaSauHabitat.jpg</t>
+  </si>
+  <si>
     <t>64</t>
   </si>
   <si>
@@ -92,6 +107,9 @@
     <t>35.0</t>
   </si>
   <si>
+    <t>SuTuHabitat.jpg</t>
+  </si>
+  <si>
     <t>65</t>
   </si>
   <si>
@@ -101,6 +119,9 @@
     <t>8</t>
   </si>
   <si>
+    <t>KhiHabitat.jpg</t>
+  </si>
+  <si>
     <t>66</t>
   </si>
   <si>
@@ -113,6 +134,9 @@
     <t>Tê giác</t>
   </si>
   <si>
+    <t>TeGiacHabitat.jpg</t>
+  </si>
+  <si>
     <t>68</t>
   </si>
   <si>
@@ -125,6 +149,9 @@
     <t>10</t>
   </si>
   <si>
+    <t>HongHacHabiat.jpg</t>
+  </si>
+  <si>
     <t>69</t>
   </si>
   <si>
@@ -132,6 +159,9 @@
   </si>
   <si>
     <t>55.0</t>
+  </si>
+  <si>
+    <t>SoiHabitat.jpeg</t>
   </si>
 </sst>
 </file>
@@ -219,7 +249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -230,6 +260,7 @@
     <col min="3" max="3" width="18.1640625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="21.31640625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="19.3125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="23.68359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -248,192 +279,228 @@
       <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>12</v>
-      </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F7" t="s" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="F9" t="s" s="2">
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="F10" t="s" s="2">
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="F11" t="s" s="2">
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F12" t="s" s="2">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>